<commit_message>
double resonator far field
</commit_message>
<xml_diff>
--- a/variables.xlsx
+++ b/variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Non-Hermitian Gauge Field\non-hermitian-gauge-field\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E5C180-E848-4C24-A7CD-8697A5F5C00E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF753A2-3C51-4F68-8792-28C05D9F7391}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="852" yWindow="-108" windowWidth="22296" windowHeight="13176" tabRatio="1000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1560,7 +1560,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1713,8 +1713,8 @@
         <v>16</v>
       </c>
       <c r="B14" s="18">
-        <f>500*10^-9</f>
-        <v>5.0000000000000008E-7</v>
+        <f>100*10^-9</f>
+        <v>1.0000000000000001E-7</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
@@ -1870,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G15" sqref="B10:G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1913,23 +1913,23 @@
       <c r="A2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B2">
-        <v>0.99115050000000005</v>
-      </c>
-      <c r="C2">
-        <v>0.98237931499999998</v>
-      </c>
-      <c r="D2">
-        <v>0.97368574900000004</v>
-      </c>
-      <c r="E2">
-        <v>0.96506911799999995</v>
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0</v>
       </c>
       <c r="F2" s="6">
-        <v>0.95652873900000002</v>
+        <v>0</v>
       </c>
       <c r="G2" s="6">
-        <v>0.94806393799999999</v>
+        <v>0</v>
       </c>
       <c r="H2" s="6">
         <v>0</v>
@@ -1942,23 +1942,23 @@
       <c r="A3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="15">
-        <v>0.90700000000000003</v>
-      </c>
-      <c r="D3">
-        <v>0.91494722900000003</v>
-      </c>
-      <c r="E3">
-        <v>0.92311634600000003</v>
+      <c r="B3" s="6">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0</v>
       </c>
       <c r="F3" s="6">
-        <v>0.93135840199999997</v>
+        <v>0</v>
       </c>
       <c r="G3" s="6">
-        <v>0.93967404700000001</v>
+        <v>0</v>
       </c>
       <c r="H3" s="6">
         <v>0</v>
@@ -2004,23 +2004,23 @@
       <c r="A4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B4">
-        <v>0.93135840199999997</v>
-      </c>
-      <c r="C4">
-        <v>0.97368574900000004</v>
-      </c>
-      <c r="D4">
-        <v>0.96506911799999995</v>
-      </c>
-      <c r="E4">
-        <v>0.95652873900000002</v>
+      <c r="B4" s="6">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0</v>
       </c>
       <c r="F4" s="6">
-        <v>0.94806393799999999</v>
+        <v>0</v>
       </c>
       <c r="G4" s="6">
-        <v>0.93967404700000001</v>
+        <v>0</v>
       </c>
       <c r="H4" s="6">
         <v>0</v>
@@ -2066,23 +2066,23 @@
       <c r="A5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B5">
-        <v>0.93967404700000001</v>
-      </c>
-      <c r="C5">
-        <v>0.898825231</v>
-      </c>
-      <c r="D5">
-        <v>0.90685040400000005</v>
-      </c>
-      <c r="E5" s="15">
-        <v>0.91500000000000004</v>
+      <c r="B5" s="6">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0</v>
       </c>
       <c r="F5" s="6">
-        <v>0.92311634600000003</v>
+        <v>0</v>
       </c>
       <c r="G5" s="6">
-        <v>0.93135840199999997</v>
+        <v>0</v>
       </c>
       <c r="H5" s="6">
         <v>0</v>
@@ -2129,22 +2129,22 @@
         <v>53</v>
       </c>
       <c r="B6" s="6">
-        <v>0.87517331899999995</v>
+        <v>0</v>
       </c>
       <c r="C6" s="6">
-        <v>0.96506911799999995</v>
+        <v>0</v>
       </c>
       <c r="D6" s="6">
-        <v>0.95652873900000002</v>
+        <v>0</v>
       </c>
       <c r="E6" s="6">
-        <v>0.94806393799999999</v>
+        <v>0</v>
       </c>
       <c r="F6" s="6">
-        <v>0.93967404700000001</v>
+        <v>0</v>
       </c>
       <c r="G6" s="6">
-        <v>0.93135840199999997</v>
+        <v>0</v>
       </c>
       <c r="H6" s="6">
         <v>0</v>
@@ -2191,22 +2191,22 @@
         <v>54</v>
       </c>
       <c r="B7" s="6">
-        <v>0.88298731500000005</v>
+        <v>0</v>
       </c>
       <c r="C7" s="6">
-        <v>0.89087107799999998</v>
+        <v>0</v>
       </c>
       <c r="D7" s="6">
-        <v>0.898825231</v>
+        <v>0</v>
       </c>
       <c r="E7" s="6">
-        <v>0.90685040400000005</v>
+        <v>0</v>
       </c>
       <c r="F7" s="6">
-        <v>0.91494722900000003</v>
+        <v>0</v>
       </c>
       <c r="G7" s="6">
-        <v>0.92311634600000003</v>
+        <v>0</v>
       </c>
       <c r="H7" s="6">
         <v>0</v>
@@ -2269,23 +2269,23 @@
       <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B10">
-        <v>1.570796327</v>
-      </c>
-      <c r="C10" s="15">
-        <v>3.1415926540000001</v>
-      </c>
-      <c r="D10" s="15">
-        <v>-1.570796327</v>
-      </c>
-      <c r="E10" s="15">
-        <v>-4.2100000000000002E-15</v>
+      <c r="B10" s="6">
+        <v>0</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0</v>
       </c>
       <c r="F10" s="6">
-        <v>1.570796327</v>
+        <v>0</v>
       </c>
       <c r="G10" s="6">
-        <v>3.1415926540000001</v>
+        <v>0</v>
       </c>
       <c r="H10" s="6">
         <v>0</v>
@@ -2322,23 +2322,23 @@
       <c r="A11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11" s="15">
-        <v>-1.570796327</v>
-      </c>
-      <c r="D11" s="15">
-        <v>3.14</v>
-      </c>
-      <c r="E11">
-        <v>1.570796327</v>
-      </c>
-      <c r="F11" s="14">
-        <v>-4.7099999999999996E-15</v>
+      <c r="B11" s="6">
+        <v>0</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0</v>
       </c>
       <c r="G11" s="6">
-        <v>-1.570796327</v>
+        <v>0</v>
       </c>
       <c r="H11" s="6">
         <v>0</v>
@@ -2372,23 +2372,23 @@
       <c r="A12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B12">
-        <v>-1.570796327</v>
-      </c>
-      <c r="C12" s="15">
-        <v>-3.37E-16</v>
-      </c>
-      <c r="D12" s="15">
-        <v>1.570796327</v>
-      </c>
-      <c r="E12" s="15">
-        <v>3.14</v>
+      <c r="B12" s="6">
+        <v>0</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0</v>
       </c>
       <c r="F12" s="6">
-        <v>-1.570796327</v>
-      </c>
-      <c r="G12" s="14">
-        <v>-3.6899999999999996E-15</v>
+        <v>0</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0</v>
       </c>
       <c r="H12" s="6">
         <v>0</v>
@@ -2422,23 +2422,23 @@
       <c r="A13" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B13">
-        <v>3.1415926540000001</v>
-      </c>
-      <c r="C13" s="15">
-        <v>1.570796327</v>
-      </c>
-      <c r="D13" s="15">
-        <v>-4.0899999999999998E-15</v>
-      </c>
-      <c r="E13" s="15">
-        <v>-1.570796327</v>
+      <c r="B13" s="6">
+        <v>0</v>
+      </c>
+      <c r="C13" s="6">
+        <v>0</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0</v>
+      </c>
+      <c r="E13" s="6">
+        <v>0</v>
       </c>
       <c r="F13" s="6">
-        <v>-3.1415926540000001</v>
+        <v>0</v>
       </c>
       <c r="G13" s="6">
-        <v>1.570796327</v>
+        <v>0</v>
       </c>
       <c r="H13" s="6">
         <v>0</v>
@@ -2473,22 +2473,22 @@
         <v>53</v>
       </c>
       <c r="B14" s="6">
-        <v>1.570796327</v>
+        <v>0</v>
       </c>
       <c r="C14" s="6">
-        <v>3.1415926540000001</v>
+        <v>0</v>
       </c>
       <c r="D14" s="6">
-        <v>-1.570796327</v>
-      </c>
-      <c r="E14" s="14">
-        <v>-1.8599999999999999E-16</v>
+        <v>0</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0</v>
       </c>
       <c r="F14" s="6">
-        <v>1.570796327</v>
+        <v>0</v>
       </c>
       <c r="G14" s="6">
-        <v>3.1415926540000001</v>
+        <v>0</v>
       </c>
       <c r="H14" s="6">
         <v>0</v>
@@ -2498,23 +2498,23 @@
       <c r="A15" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="14">
-        <v>2.1499999999999999E-16</v>
+      <c r="B15" s="6">
+        <v>0</v>
       </c>
       <c r="C15" s="6">
-        <v>-1.570796327</v>
+        <v>0</v>
       </c>
       <c r="D15" s="6">
-        <v>3.1415926540000001</v>
+        <v>0</v>
       </c>
       <c r="E15" s="6">
-        <v>1.570796327</v>
-      </c>
-      <c r="F15" s="14">
-        <v>-2.9200000000000001E-15</v>
+        <v>0</v>
+      </c>
+      <c r="F15" s="6">
+        <v>0</v>
       </c>
       <c r="G15" s="6">
-        <v>-1.570796327</v>
+        <v>0</v>
       </c>
       <c r="H15" s="6">
         <v>0</v>

</xml_diff>